<commit_message>
Bug Fixes and Code Cleanup
> Got bar bin sizes working.
> Reorganized code, and removed additional unnecessary code
> Other minor fixes
> The new excel file labeled w Pivot (maybe also in previous change),
has excel graphs that match the graphs in this webpage.  This was just a
tool to check that the results being displayed were accurate.

With more work, I think it would be possible to graph two lines of
average $/kw.  There is a compoundChart type in dc that allows you to
overlay charts, which is how you can get multiple lines into a chart.
Also, to do a reduceAverage in crossfilter, you need to build a custom
reduce funciton using reduce().  I read some stuff and saw an example on
the internet of how to do a reduce Average, might take a day to figure
out.

>
</commit_message>
<xml_diff>
--- a/line/cdp8_modifiedHeaders_wPivot.xlsx
+++ b/line/cdp8_modifiedHeaders_wPivot.xlsx
@@ -4,24 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="96" windowWidth="15312" windowHeight="11052" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="96" windowWidth="15312" windowHeight="11052" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BarChartCapacity" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId2"/>
-    <sheet name="RawData" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Capacity by value" sheetId="6" r:id="rId2"/>
+    <sheet name="Stations built over time" sheetId="7" r:id="rId3"/>
+    <sheet name="RawData" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>year</t>
   </si>
@@ -51,6 +50,9 @@
   </si>
   <si>
     <t>Count of year</t>
+  </si>
+  <si>
+    <t>Count of capacity_kW</t>
   </si>
 </sst>
 </file>
@@ -272,11 +274,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="67765376"/>
-        <c:axId val="67766912"/>
+        <c:axId val="84155008"/>
+        <c:axId val="84160896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67765376"/>
+        <c:axId val="84155008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -285,7 +287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67766912"/>
+        <c:crossAx val="84160896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -293,7 +295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67766912"/>
+        <c:axId val="84160896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,7 +306,241 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67765376"/>
+        <c:crossAx val="84155008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[cdp8_modifiedHeaders_wPivot.xlsx]Stations built over time!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stations constructed over time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Stations built over time'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Stations built over time'!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stations built over time'!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="95062272"/>
+        <c:axId val="95064064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="95062272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95064064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95064064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95062272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -372,6 +608,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="NREL" refreshedDate="42200.759929976855" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="390">
   <cacheSource type="worksheet">
@@ -379,7 +650,21 @@
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="year" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2002" maxValue="2014"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2002" maxValue="2014" count="13">
+        <n v="2010"/>
+        <n v="2007"/>
+        <n v="2009"/>
+        <n v="2011"/>
+        <n v="2012"/>
+        <n v="2013"/>
+        <n v="2014"/>
+        <n v="2008"/>
+        <n v="2004"/>
+        <n v="2005"/>
+        <n v="2006"/>
+        <n v="2003"/>
+        <n v="2002"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="capacity_kW" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="5" maxValue="4200" count="38">
@@ -456,7 +741,7 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="390">
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <n v="5651130"/>
@@ -465,7 +750,7 @@
     <n v="814.08108108108104"/>
   </r>
   <r>
-    <n v="2007"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <n v="4004512.0822199401"/>
@@ -474,7 +759,7 @@
     <n v="7411.0746557040102"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="2"/>
     <x v="2"/>
     <n v="4405901.8959999997"/>
@@ -483,7 +768,7 @@
     <n v="6538.4469920000001"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
     <n v="4357368.4000000004"/>
@@ -492,7 +777,7 @@
     <n v="5833.4210000000003"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="3"/>
     <x v="1"/>
     <n v="2385664.5120000001"/>
@@ -501,7 +786,7 @@
     <n v="6868.3225599999996"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="4"/>
     <x v="1"/>
     <n v="1012000"/>
@@ -510,7 +795,7 @@
     <n v="7084"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
     <n v="5267214.0839999998"/>
@@ -519,7 +804,7 @@
     <n v="8108.03521"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
     <n v="5267214.0839999998"/>
@@ -528,7 +813,7 @@
     <n v="8108.03521"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
     <n v="5267214.0839999998"/>
@@ -537,7 +822,7 @@
     <n v="9373.03521"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5650400"/>
@@ -546,7 +831,7 @@
     <n v="6300.8"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4475980"/>
@@ -555,7 +840,7 @@
     <n v="5895.1904761904798"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3353906"/>
@@ -564,7 +849,7 @@
     <n v="6179.6866666666701"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="4439031"/>
@@ -573,7 +858,7 @@
     <n v="6097.5775000000003"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="7"/>
     <x v="2"/>
     <n v="6743530"/>
@@ -582,7 +867,7 @@
     <n v="6239.2166666666699"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3378539"/>
@@ -591,7 +876,7 @@
     <n v="6261.7966666666698"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3353906"/>
@@ -600,7 +885,7 @@
     <n v="6179.6866666666701"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3347255"/>
@@ -609,7 +894,7 @@
     <n v="6157.5166666666701"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3366223"/>
@@ -618,7 +903,7 @@
     <n v="6220.7433333333302"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5412500"/>
@@ -627,7 +912,7 @@
     <n v="5825"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="8"/>
     <x v="2"/>
     <n v="8943750"/>
@@ -636,7 +921,7 @@
     <n v="6179.6875"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="4397976"/>
@@ -645,7 +930,7 @@
     <n v="5994.94"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="7"/>
     <x v="2"/>
     <n v="6596964"/>
@@ -654,7 +939,7 @@
     <n v="5994.94"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="5462760"/>
@@ -663,7 +948,7 @@
     <n v="13209.2"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="7"/>
     <x v="2"/>
     <n v="6763758"/>
@@ -672,7 +957,7 @@
     <n v="8272.93"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5203430"/>
@@ -681,7 +966,7 @@
     <n v="5406.86"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="3"/>
     <x v="1"/>
     <n v="2227727"/>
@@ -690,7 +975,7 @@
     <n v="6138.6350000000002"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="3"/>
     <x v="1"/>
     <n v="2227727"/>
@@ -699,7 +984,7 @@
     <n v="6138.6350000000002"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5606476"/>
@@ -708,7 +993,7 @@
     <n v="6212.9520000000002"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="9"/>
     <x v="1"/>
     <n v="4069027"/>
@@ -717,7 +1002,7 @@
     <n v="6302.8527777777799"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3353906"/>
@@ -726,7 +1011,7 @@
     <n v="6179.6866666666701"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3366223"/>
@@ -735,7 +1020,7 @@
     <n v="6220.7433333333302"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1989998"/>
@@ -744,7 +1029,7 @@
     <n v="4476.1809523809497"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1979734"/>
@@ -753,7 +1038,7 @@
     <n v="4427.3047619047602"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2826846"/>
@@ -762,7 +1047,7 @@
     <n v="10461.171428571401"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="0"/>
     <n v="10880903"/>
@@ -771,7 +1056,7 @@
     <n v="7434.19333333334"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="12"/>
     <x v="2"/>
     <n v="5599460"/>
@@ -780,7 +1065,7 @@
     <n v="5888.0317460317501"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="13"/>
     <x v="1"/>
     <n v="1136789"/>
@@ -789,7 +1074,7 @@
     <n v="7826.5619047619102"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2110849"/>
@@ -798,7 +1083,7 @@
     <n v="7051.6619047619097"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="5591950"/>
@@ -807,7 +1092,7 @@
     <n v="8314.1666666666697"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4213701"/>
@@ -816,7 +1101,7 @@
     <n v="7032.6214285714304"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="13"/>
     <x v="1"/>
     <n v="1053424"/>
@@ -825,7 +1110,7 @@
     <n v="7032.6095238095204"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="750000"/>
@@ -834,7 +1119,7 @@
     <n v="571.42857142857099"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="6072163"/>
@@ -843,7 +1128,7 @@
     <n v="10180.407499999999"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4931757"/>
@@ -852,7 +1137,7 @@
     <n v="6742.2785714285701"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6318081"/>
@@ -861,7 +1146,7 @@
     <n v="7028.7"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11220743"/>
@@ -870,7 +1155,7 @@
     <n v="7757.8504761904796"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4471875"/>
@@ -879,7 +1164,7 @@
     <n v="7647.3214285714303"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6707813"/>
@@ -888,7 +1173,7 @@
     <n v="7647.3222222222203"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11179688"/>
@@ -897,7 +1182,7 @@
     <n v="7718.7504761904802"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11179688"/>
@@ -906,7 +1191,7 @@
     <n v="7718.7504761904802"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6141146"/>
@@ -915,7 +1200,7 @@
     <n v="6747.8507936507904"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4094097"/>
@@ -924,7 +1209,7 @@
     <n v="6747.85"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5098718.5517908996"/>
@@ -933,7 +1218,7 @@
     <n v="5299.08279574056"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="13915402.644724101"/>
@@ -942,7 +1227,7 @@
     <n v="10670.3520324529"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="5"/>
     <x v="1"/>
     <n v="5085972.05421104"/>
@@ -951,7 +1236,7 @@
     <n v="9464.3459456967703"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12870344.631171299"/>
@@ -960,7 +1245,7 @@
     <n v="9675.0586862121399"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="5"/>
     <x v="1"/>
     <n v="3267912.58470474"/>
@@ -969,7 +1254,7 @@
     <n v="5292.3802609136601"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6365392.8092933204"/>
@@ -978,7 +1263,7 @@
     <n v="9479.4464057530095"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6365392.8092933204"/>
@@ -987,7 +1272,7 @@
     <n v="9479.4464057530095"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12005478.4588577"/>
@@ -996,7 +1281,7 @@
     <n v="8851.6565233024503"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4840495.9264278803"/>
@@ -1005,7 +1290,7 @@
     <n v="8879.8789747844894"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="12"/>
     <x v="2"/>
     <n v="7616326.6950629205"/>
@@ -1014,7 +1299,7 @@
     <n v="9444.2961262465597"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="15"/>
     <x v="1"/>
     <n v="4794047.7715392103"/>
@@ -1023,7 +1308,7 @@
     <n v="12574.087948493399"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2551241.22362052"/>
@@ -1032,7 +1317,7 @@
     <n v="9503.6564052920294"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="5"/>
     <x v="1"/>
     <n v="5618624"/>
@@ -1041,7 +1326,7 @@
     <n v="10732.5648642419"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="16"/>
     <x v="2"/>
     <n v="10271494.3426912"/>
@@ -1050,7 +1335,7 @@
     <n v="9582.8581293504794"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="5"/>
     <x v="1"/>
     <n v="5542280.20909971"/>
@@ -1059,7 +1344,7 @@
     <n v="10550.7939335269"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12748861.5256534"/>
@@ -1068,7 +1353,7 @@
     <n v="9559.6403964412493"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="17"/>
     <x v="1"/>
     <n v="4588950.5551330801"/>
@@ -1077,7 +1362,7 @@
     <n v="9064.5435668008195"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12440165.8403042"/>
@@ -1086,7 +1371,7 @@
     <n v="9312.0051276480208"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2538063.2927756701"/>
@@ -1095,7 +1380,7 @@
     <n v="9488.6772768422998"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="5"/>
     <x v="1"/>
     <n v="5205520.2129277596"/>
@@ -1104,7 +1389,7 @@
     <n v="9796.7573420242607"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="12"/>
     <x v="2"/>
     <n v="7698509.7319587599"/>
@@ -1113,7 +1398,7 @@
     <n v="10000.655931926"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11573557.319587599"/>
@@ -1122,7 +1407,7 @@
     <n v="8766.7418753068196"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11714998.309278401"/>
@@ -1131,7 +1416,7 @@
     <n v="8901.4475797741798"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6236743.5463917498"/>
@@ -1140,7 +1425,7 @@
     <n v="9569.0785272459507"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6240617.0309278397"/>
@@ -1149,7 +1434,7 @@
     <n v="9576.4565930289591"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="10587511.752577299"/>
@@ -1158,7 +1443,7 @@
     <n v="7827.6508591065303"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6358939.4639175301"/>
@@ -1167,7 +1452,7 @@
     <n v="9801.8326558664703"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="15"/>
     <x v="1"/>
     <n v="4065486.63917526"/>
@@ -1176,7 +1461,7 @@
     <n v="10595.873801341801"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="15"/>
     <x v="1"/>
     <n v="4193294.5567010301"/>
@@ -1185,7 +1470,7 @@
     <n v="9294.3967272132195"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="15"/>
     <x v="1"/>
     <n v="4229489.4432989703"/>
@@ -1194,7 +1479,7 @@
     <n v="9409.3011291114399"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4984678.5567010297"/>
@@ -1203,7 +1488,7 @@
     <n v="9557.8492881688799"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="13393858.8865979"/>
@@ -1212,7 +1497,7 @@
     <n v="10500.3624153166"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="13393858.8865979"/>
@@ -1221,7 +1506,7 @@
     <n v="10500.3624153166"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="14"/>
     <x v="2"/>
     <n v="7467427.5682656802"/>
@@ -1230,7 +1515,7 @@
     <n v="12173.5313371991"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6559404.9667896703"/>
@@ -1239,7 +1524,7 @@
     <n v="10443.964477244799"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="11"/>
     <x v="0"/>
     <n v="13085527.830258301"/>
@@ -1248,7 +1533,7 @@
     <n v="10460.813361447899"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6635981.8118081205"/>
@@ -1257,7 +1542,7 @@
     <n v="10589.825134422799"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="18"/>
     <x v="3"/>
     <n v="41880555.719557203"/>
@@ -1266,7 +1551,7 @@
     <n v="8860.1569144262903"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1275,7 +1560,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1284,7 +1569,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1293,7 +1578,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1302,7 +1587,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1311,7 +1596,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1320,7 +1605,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1329,7 +1614,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1338,7 +1623,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1347,7 +1632,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1356,7 +1641,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1365,7 +1650,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1374,7 +1659,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1383,7 +1668,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1392,7 +1677,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1401,7 +1686,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2897596.8634686298"/>
@@ -1410,7 +1695,7 @@
     <n v="11747.940080829399"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1419,7 +1704,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1428,7 +1713,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1437,7 +1722,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1446,7 +1731,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1455,7 +1740,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3808387.5276752799"/>
@@ -1464,7 +1749,7 @@
     <n v="10039.9789140749"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1473,7 +1758,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1482,7 +1767,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1491,7 +1776,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1500,7 +1785,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1509,7 +1794,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1518,7 +1803,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -1527,7 +1812,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6105026.3025830304"/>
@@ -1536,7 +1821,7 @@
     <n v="9578.4813073273599"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="6"/>
     <x v="1"/>
     <n v="2909922.0040000002"/>
@@ -1545,7 +1830,7 @@
     <n v="6663.7400133333304"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="2700000"/>
@@ -1554,7 +1839,7 @@
     <n v="4000"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2244149"/>
@@ -1563,7 +1848,7 @@
     <n v="5686.4238095238097"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="2700000"/>
@@ -1572,7 +1857,7 @@
     <n v="4000"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4521141"/>
@@ -1581,7 +1866,7 @@
     <n v="5764.6214285714304"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="2700000"/>
@@ -1590,7 +1875,7 @@
     <n v="1750"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="2700000"/>
@@ -1599,7 +1884,7 @@
     <n v="1750"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11138633"/>
@@ -1608,7 +1893,7 @@
     <n v="5727.2695238095303"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <n v="4100660"/>
@@ -1617,7 +1902,7 @@
     <n v="5201.32"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="7"/>
     <x v="2"/>
     <n v="6683180"/>
@@ -1626,7 +1911,7 @@
     <n v="6138.6333333333296"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11220743"/>
@@ -1635,7 +1920,7 @@
     <n v="5805.4695238095301"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6732446"/>
@@ -1644,7 +1929,7 @@
     <n v="5686.4222222222197"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3954256"/>
@@ -1653,7 +1938,7 @@
     <n v="7553.1936507936498"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="16"/>
     <x v="2"/>
     <n v="8910906"/>
@@ -1662,7 +1947,7 @@
     <n v="5608.2214285714299"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="14"/>
     <x v="2"/>
     <n v="5569316"/>
@@ -1671,7 +1956,7 @@
     <n v="7608.2209523809497"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3341590"/>
@@ -1680,7 +1965,7 @@
     <n v="7608.2222222222199"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3341590"/>
@@ -1689,7 +1974,7 @@
     <n v="7608.2222222222199"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="16"/>
     <x v="2"/>
     <n v="8927328"/>
@@ -1698,7 +1983,7 @@
     <n v="7627.7714285714301"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="3327920"/>
@@ -1707,7 +1992,7 @@
     <n v="4923.6190476190504"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="14360135.0087125"/>
@@ -1716,7 +2001,7 @@
     <n v="11093.9066648228"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12359584.410455"/>
@@ -1725,7 +2010,7 @@
     <n v="9188.6203807679904"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="14320409.355275899"/>
@@ -1734,7 +2019,7 @@
     <n v="11056.0727091689"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6726820.7566539897"/>
@@ -1743,7 +2028,7 @@
     <n v="8080.1548614883204"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2373575.7756654001"/>
@@ -1752,7 +2037,7 @@
     <n v="8705.4033858410294"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3363410.85931559"/>
@@ -1761,7 +2046,7 @@
     <n v="8080.1563884362404"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="14"/>
     <x v="2"/>
     <n v="5605683.4828897296"/>
@@ -1770,7 +2055,7 @@
     <n v="8080.1539453195701"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2258126.0076045599"/>
@@ -1779,7 +2064,7 @@
     <n v="8155.6425855513298"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6703129.1825095098"/>
@@ -1788,7 +2073,7 @@
     <n v="8042.5491882430997"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2802618.56273764"/>
@@ -1797,7 +2082,7 @@
     <n v="10748.4642766612"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -1806,7 +2091,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2242273.5855513299"/>
@@ -1815,7 +2100,7 @@
     <n v="8080.1548614883204"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2242273.5855513299"/>
@@ -1824,7 +2109,7 @@
     <n v="8080.1548614883204"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2242273.5855513299"/>
@@ -1833,7 +2118,7 @@
     <n v="8080.1548614883204"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -1842,7 +2127,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -1851,7 +2136,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2218493.5095056999"/>
@@ -1860,7 +2145,7 @@
     <n v="7966.9164041281902"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -1869,7 +2154,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -1878,7 +2163,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -1887,7 +2172,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -1896,7 +2181,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2258126.9695817502"/>
@@ -1905,7 +2190,7 @@
     <n v="8155.6471663950797"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="12"/>
     <x v="2"/>
     <n v="7657166.2091254797"/>
@@ -1914,7 +2199,7 @@
     <n v="9556.8936749351196"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="5"/>
     <x v="1"/>
     <n v="5118189.5257732002"/>
@@ -1923,7 +2208,7 @@
     <n v="9875.7325478645107"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="14"/>
     <x v="2"/>
     <n v="7122696.9072164996"/>
@@ -1932,7 +2217,7 @@
     <n v="11256.608738340699"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="19"/>
     <x v="1"/>
     <n v="6547712.0824742299"/>
@@ -1941,7 +2226,7 @@
     <n v="11547.158719249401"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="15"/>
     <x v="1"/>
     <n v="4217322.6804123698"/>
@@ -1950,7 +2235,7 @@
     <n v="9370.6764850269992"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2347281.36082474"/>
@@ -1959,7 +2244,7 @@
     <n v="7159.8808051055503"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="13913327.876288701"/>
@@ -1968,7 +2253,7 @@
     <n v="10995.0947864507"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="20"/>
     <x v="1"/>
     <n v="3689513.9381443299"/>
@@ -1977,7 +2262,7 @@
     <n v="11744.858203240099"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="20"/>
     <x v="1"/>
     <n v="3436482.63917526"/>
@@ -1986,7 +2271,7 @@
     <n v="10780.9294452626"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="21"/>
     <x v="1"/>
     <n v="4982793.0309278397"/>
@@ -1995,7 +2280,7 @@
     <n v="10344.2794698085"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -2004,7 +2289,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2013,7 +2298,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2022,7 +2307,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2031,7 +2316,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2040,7 +2325,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2049,7 +2334,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2058,7 +2343,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2067,7 +2352,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2076,7 +2361,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2085,7 +2370,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2094,7 +2379,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2103,7 +2388,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2112,7 +2397,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2121,7 +2406,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2190177.1217712201"/>
@@ -2130,7 +2415,7 @@
     <n v="8379.2746441750096"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="20"/>
     <x v="1"/>
     <n v="4854178.4317343198"/>
@@ -2139,7 +2424,7 @@
     <n v="16441.968089966598"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3485910.5535055399"/>
@@ -2148,7 +2433,7 @@
     <n v="9016.2424881391707"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3485910.5535055399"/>
@@ -2157,7 +2442,7 @@
     <n v="9016.2424881391707"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="20"/>
     <x v="1"/>
     <n v="2914686.9667896698"/>
@@ -2166,7 +2451,7 @@
     <n v="9053.4291758917607"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2323940.3690036898"/>
@@ -2175,7 +2460,7 @@
     <n v="9016.2424881391707"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2331749.7601476"/>
@@ -2184,7 +2469,7 @@
     <n v="9053.4300650149307"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2355177.9335793401"/>
@@ -2193,7 +2478,7 @@
     <n v="9164.9927956422398"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2323940.3690036898"/>
@@ -2202,7 +2487,7 @@
     <n v="9016.2424881391707"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="14"/>
     <x v="2"/>
     <n v="1966911.62361624"/>
@@ -2211,7 +2496,7 @@
     <n v="1696.35810929538"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2220,7 +2505,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2229,7 +2514,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2238,7 +2523,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2247,7 +2532,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2256,7 +2541,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2265,7 +2550,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2274,7 +2559,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2283,7 +2568,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2292,7 +2577,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2301,7 +2586,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2310,7 +2595,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2319,7 +2604,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2328,7 +2613,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="1966911.62361624"/>
@@ -2337,7 +2622,7 @@
     <n v="7316.1056053417697"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="4"/>
     <x v="1"/>
     <n v="1130285"/>
@@ -2346,7 +2631,7 @@
     <n v="6302.85"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="22"/>
     <x v="2"/>
     <n v="10172567"/>
@@ -2355,7 +2640,7 @@
     <n v="6302.85222222222"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="23"/>
     <x v="0"/>
     <n v="9111573"/>
@@ -2364,7 +2649,7 @@
     <n v="4111.5730000000003"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5782335"/>
@@ -2373,7 +2658,7 @@
     <n v="8564.67"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4899383"/>
@@ -2382,7 +2667,7 @@
     <n v="6665.1976190476198"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4899383"/>
@@ -2391,7 +2676,7 @@
     <n v="6665.1976190476198"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4917865"/>
@@ -2400,7 +2685,7 @@
     <n v="6709.2023809523798"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4899383"/>
@@ -2409,7 +2694,7 @@
     <n v="6665.1976190476198"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="5"/>
     <x v="1"/>
     <n v="3600000"/>
@@ -2418,7 +2703,7 @@
     <n v="5571.4285714285697"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="24"/>
     <x v="2"/>
     <n v="4410000"/>
@@ -2427,7 +2712,7 @@
     <n v="3428.5714285714298"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="20"/>
     <x v="1"/>
     <n v="3566739.6282671802"/>
@@ -2436,7 +2721,7 @@
     <n v="10942.4682100217"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2551241.22362052"/>
@@ -2445,7 +2730,7 @@
     <n v="9503.6564052920294"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11211367.927756701"/>
@@ -2454,7 +2739,7 @@
     <n v="8141.9962520369399"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6726144.4866920197"/>
@@ -2463,7 +2748,7 @@
     <n v="8079.0814171042302"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="5"/>
     <x v="1"/>
     <n v="4340941.2927756701"/>
@@ -2472,7 +2757,7 @@
     <n v="7738.2361035669001"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="14"/>
     <x v="2"/>
     <n v="5605946.1026616003"/>
@@ -2481,7 +2766,7 @@
     <n v="8080.6541734564598"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6649186.3117870698"/>
@@ -2490,7 +2775,7 @@
     <n v="10067.7783813145"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3363410.85931559"/>
@@ -2499,7 +2784,7 @@
     <n v="8080.1563884362404"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="12"/>
     <x v="2"/>
     <n v="6679261.5665399302"/>
@@ -2508,7 +2793,7 @@
     <n v="8004.6640835294802"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3878692.01520913"/>
@@ -2517,7 +2802,7 @@
     <n v="9715.9695817490501"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12336395.437262399"/>
@@ -2526,7 +2811,7 @@
     <n v="9213.1761723700893"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="11"/>
     <x v="0"/>
     <n v="13298372.6235741"/>
@@ -2535,7 +2820,7 @@
     <n v="10129.3449212385"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="25"/>
     <x v="2"/>
     <n v="9522473.6425855495"/>
@@ -2544,7 +2829,7 @@
     <n v="9494.6916192890294"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11746598.8865979"/>
@@ -2553,7 +2838,7 @@
     <n v="8931.5433676976008"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12392840.0824742"/>
@@ -2562,7 +2847,7 @@
     <n v="9547.0111732940604"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="25"/>
     <x v="2"/>
     <n v="8733167.3402061891"/>
@@ -2571,7 +2856,7 @@
     <n v="8779.3033153330107"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3793814.43298969"/>
@@ -2580,7 +2865,7 @@
     <n v="9733.4223531336902"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6518272.0824742299"/>
@@ -2589,7 +2874,7 @@
     <n v="10105.323357879201"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -2598,7 +2883,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2897596.8634686298"/>
@@ -2607,7 +2892,7 @@
     <n v="11747.940080829399"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -2616,7 +2901,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6152525.8856088603"/>
@@ -2625,7 +2910,7 @@
     <n v="9668.9567035670407"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12138593.6420664"/>
@@ -2634,7 +2919,7 @@
     <n v="9558.9712774556301"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -2643,7 +2928,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -2652,7 +2937,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="5"/>
     <x v="1"/>
     <n v="5217962.5571955703"/>
@@ -2661,7 +2946,7 @@
     <n v="10373.580152873001"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3509338.7269372698"/>
@@ -2670,7 +2955,7 @@
     <n v="9090.6176418907107"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2227727"/>
@@ -2679,7 +2964,7 @@
     <n v="5608.2238095238099"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="6"/>
     <x v="1"/>
     <n v="3341590"/>
@@ -2688,7 +2973,7 @@
     <n v="6138.6333333333296"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2227727"/>
@@ -2697,7 +2982,7 @@
     <n v="5608.2238095238099"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="3486506"/>
@@ -2706,7 +2991,7 @@
     <n v="3716.2649999999999"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="7"/>
     <x v="2"/>
     <n v="5182963"/>
@@ -2715,7 +3000,7 @@
     <n v="3638.2716666666702"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="15"/>
     <x v="1"/>
     <n v="3341590"/>
@@ -2724,7 +3009,7 @@
     <n v="7608.2222222222199"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11138643"/>
@@ -2733,7 +3018,7 @@
     <n v="7679.66"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11983736.623426899"/>
@@ -2742,7 +3027,7 @@
     <n v="8830.6701074079192"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2226420.20152091"/>
@@ -2751,7 +3036,7 @@
     <n v="8004.6625565815702"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6352612.5931558898"/>
@@ -2760,7 +3045,7 @@
     <n v="9502.8760601122594"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="14"/>
     <x v="2"/>
     <n v="6170812.3726235703"/>
@@ -2769,7 +3054,7 @@
     <n v="7232.6355531414101"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="15"/>
     <x v="1"/>
     <n v="4367424"/>
@@ -2778,7 +3063,7 @@
     <n v="11554.405105547399"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="11"/>
     <x v="0"/>
     <n v="12407796.247422701"/>
@@ -2787,7 +3072,7 @@
     <n v="9561.2551399116401"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2519851.5463917502"/>
@@ -2796,7 +3081,7 @@
     <n v="9688.8600883652398"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2519851.5463917502"/>
@@ -2805,7 +3090,7 @@
     <n v="9688.8600883652398"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2519851.5463917502"/>
@@ -2814,7 +3099,7 @@
     <n v="9688.8600883652398"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2519851.5463917502"/>
@@ -2823,7 +3108,7 @@
     <n v="9688.8600883652398"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2519851.5463917502"/>
@@ -2832,7 +3117,7 @@
     <n v="9688.8600883652398"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -2841,7 +3126,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="10"/>
     <x v="1"/>
     <n v="2318077.49077491"/>
@@ -2850,7 +3135,7 @@
     <n v="8988.3240203830592"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="11"/>
     <x v="0"/>
     <n v="11837638.472324699"/>
@@ -2859,7 +3144,7 @@
     <n v="9272.3473062730609"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="20"/>
     <x v="1"/>
     <n v="2914686.9667896698"/>
@@ -2868,7 +3153,7 @@
     <n v="9053.4291758917607"/>
   </r>
   <r>
-    <n v="2008"/>
+    <x v="7"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49924.653225806498"/>
@@ -2877,7 +3162,7 @@
     <n v="7434.5274193548403"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49751.944000000003"/>
@@ -2886,7 +3171,7 @@
     <n v="7420.3887999999997"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="50024.171999999999"/>
@@ -2895,7 +3180,7 @@
     <n v="7474.8343999999997"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="50019.112000000001"/>
@@ -2904,7 +3189,7 @@
     <n v="7473.8224"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="55702.504000000001"/>
@@ -2913,7 +3198,7 @@
     <n v="8610.5007999999998"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="45540"/>
@@ -2922,7 +3207,7 @@
     <n v="6578"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="52282.955999999998"/>
@@ -2931,7 +3216,7 @@
     <n v="7926.5911999999998"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="50094"/>
@@ -2940,7 +3225,7 @@
     <n v="7488.8"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49939.163999999997"/>
@@ -2949,7 +3234,7 @@
     <n v="7457.8328000000001"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49933.091999999997"/>
@@ -2958,7 +3243,7 @@
     <n v="7456.6184000000003"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="55790.548000000003"/>
@@ -2967,7 +3252,7 @@
     <n v="8628.1095999999998"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="26"/>
     <x v="1"/>
     <n v="50094"/>
@@ -2976,7 +3261,7 @@
     <n v="7488.8"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="45000"/>
@@ -2985,7 +3270,7 @@
     <n v="6500"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="51478"/>
@@ -2994,7 +3279,7 @@
     <n v="7795.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="55055"/>
@@ -3003,7 +3288,7 @@
     <n v="8511"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="27"/>
     <x v="1"/>
     <n v="109528"/>
@@ -3012,7 +3297,7 @@
     <n v="8452.7999999999993"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49467"/>
@@ -3021,7 +3306,7 @@
     <n v="7393.4"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="55718"/>
@@ -3030,7 +3315,7 @@
     <n v="8643.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="60634"/>
@@ -3039,7 +3324,7 @@
     <n v="9626.7999999999993"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="27"/>
     <x v="1"/>
     <n v="109469"/>
@@ -3048,7 +3333,7 @@
     <n v="8446.9"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="64010"/>
@@ -3057,7 +3342,7 @@
     <n v="10302"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="54500"/>
@@ -3066,7 +3351,7 @@
     <n v="8400"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="54876"/>
@@ -3075,7 +3360,7 @@
     <n v="8475.2000000000007"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49341"/>
@@ -3084,7 +3369,7 @@
     <n v="7368.2"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="28"/>
     <x v="1"/>
     <n v="147643"/>
@@ -3093,7 +3378,7 @@
     <n v="7342.8666666666704"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61614"/>
@@ -3102,7 +3387,7 @@
     <n v="9822.7999999999993"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61400"/>
@@ -3111,7 +3396,7 @@
     <n v="9780"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61180"/>
@@ -3120,7 +3405,7 @@
     <n v="9736"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="51583"/>
@@ -3129,7 +3414,7 @@
     <n v="7816.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="27"/>
     <x v="1"/>
     <n v="89706"/>
@@ -3138,7 +3423,7 @@
     <n v="6470.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61356"/>
@@ -3147,7 +3432,7 @@
     <n v="9771.2000000000007"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="55108"/>
@@ -3156,7 +3441,7 @@
     <n v="8521.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="27"/>
     <x v="1"/>
     <n v="122278"/>
@@ -3165,7 +3450,7 @@
     <n v="9727.7999999999993"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61364"/>
@@ -3174,7 +3459,7 @@
     <n v="9772.7999999999993"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="51065"/>
@@ -3183,7 +3468,7 @@
     <n v="7713"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61352"/>
@@ -3192,7 +3477,7 @@
     <n v="9770.4"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="27"/>
     <x v="1"/>
     <n v="101138"/>
@@ -3201,7 +3486,7 @@
     <n v="7613.8"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="27"/>
     <x v="1"/>
     <n v="101138"/>
@@ -3210,7 +3495,7 @@
     <n v="7613.8"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="60247"/>
@@ -3219,7 +3504,7 @@
     <n v="9549.4"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49163"/>
@@ -3228,7 +3513,7 @@
     <n v="7332.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="29"/>
     <x v="1"/>
     <n v="188000"/>
@@ -3237,7 +3522,7 @@
     <n v="6900"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="57903"/>
@@ -3246,7 +3531,7 @@
     <n v="9080.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="27"/>
     <x v="1"/>
     <n v="122429"/>
@@ -3255,7 +3540,7 @@
     <n v="9742.9"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61088"/>
@@ -3264,7 +3549,7 @@
     <n v="9717.6"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="30"/>
     <x v="1"/>
     <n v="354944.570342205"/>
@@ -3273,7 +3558,7 @@
     <n v="12033.3341444867"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="30"/>
     <x v="1"/>
     <n v="379244.11406844098"/>
@@ -3282,7 +3567,7 @@
     <n v="13005.315893536101"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="31"/>
     <x v="0"/>
     <n v="10865484.536082501"/>
@@ -3291,7 +3576,7 @@
     <n v="7288.8659793814404"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="8"/>
     <x v="2"/>
     <n v="8153022.92783505"/>
@@ -3300,7 +3585,7 @@
     <n v="8265.9178350515504"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="54562"/>
@@ -3309,7 +3594,7 @@
     <n v="8412.4"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="56000"/>
@@ -3318,7 +3603,7 @@
     <n v="8700"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="8"/>
     <x v="2"/>
     <n v="5690721.6494845403"/>
@@ -3327,7 +3612,7 @@
     <n v="5188.0412371133998"/>
   </r>
   <r>
-    <n v="2008"/>
+    <x v="7"/>
     <x v="27"/>
     <x v="1"/>
     <n v="99848.286290322605"/>
@@ -3336,7 +3621,7 @@
     <n v="7434.4254032258104"/>
   </r>
   <r>
-    <n v="2008"/>
+    <x v="7"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49465.580645161303"/>
@@ -3345,7 +3630,7 @@
     <n v="7342.7129032258099"/>
   </r>
   <r>
-    <n v="2008"/>
+    <x v="7"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49924.653225806498"/>
@@ -3354,7 +3639,7 @@
     <n v="7434.5274193548403"/>
   </r>
   <r>
-    <n v="2008"/>
+    <x v="7"/>
     <x v="26"/>
     <x v="1"/>
     <n v="50305.173387096802"/>
@@ -3363,7 +3648,7 @@
     <n v="7510.6314516128996"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="54517"/>
@@ -3372,7 +3657,7 @@
     <n v="8403.4"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="29"/>
     <x v="1"/>
     <n v="198118"/>
@@ -3381,7 +3666,7 @@
     <n v="7405.9"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="35000"/>
@@ -3390,7 +3675,7 @@
     <n v="4500"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="55108"/>
@@ -3399,7 +3684,7 @@
     <n v="8521.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="61610"/>
@@ -3408,7 +3693,7 @@
     <n v="9822"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="56000"/>
@@ -3417,7 +3702,7 @@
     <n v="8700"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="49245"/>
@@ -3426,7 +3711,7 @@
     <n v="7349"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="68705"/>
@@ -3435,7 +3720,7 @@
     <n v="11241"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="62838"/>
@@ -3444,7 +3729,7 @@
     <n v="10067.6"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="43935"/>
@@ -3453,7 +3738,7 @@
     <n v="6287"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="54267"/>
@@ -3462,7 +3747,7 @@
     <n v="8353.4"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="26"/>
     <x v="1"/>
     <n v="47024.201355275902"/>
@@ -3471,7 +3756,7 @@
     <n v="6955.6631171345598"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="69689"/>
@@ -3480,7 +3765,7 @@
     <n v="11437.8"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="32"/>
     <x v="1"/>
     <n v="372000"/>
@@ -3489,7 +3774,7 @@
     <n v="6800"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="26"/>
     <x v="1"/>
     <n v="58035"/>
@@ -3498,7 +3783,7 @@
     <n v="9107"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="28"/>
     <x v="1"/>
     <n v="139500"/>
@@ -3507,7 +3792,7 @@
     <n v="6800"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="8"/>
     <x v="2"/>
     <n v="7022433.4600760499"/>
@@ -3516,7 +3801,7 @@
     <n v="6613.5931558935399"/>
   </r>
   <r>
-    <n v="2013"/>
+    <x v="5"/>
     <x v="33"/>
     <x v="1"/>
     <n v="1209065.8969072199"/>
@@ -3525,7 +3810,7 @@
     <n v="13187.962886597899"/>
   </r>
   <r>
-    <n v="2004"/>
+    <x v="8"/>
     <x v="23"/>
     <x v="0"/>
     <n v="8120464.0493827201"/>
@@ -3534,7 +3819,7 @@
     <n v="5326.5989629629703"/>
   </r>
   <r>
-    <n v="2004"/>
+    <x v="8"/>
     <x v="34"/>
     <x v="1"/>
     <n v="4080382.8641975299"/>
@@ -3543,7 +3828,7 @@
     <n v="13482.025283950599"/>
   </r>
   <r>
-    <n v="2005"/>
+    <x v="9"/>
     <x v="23"/>
     <x v="0"/>
     <n v="6700689.5999999996"/>
@@ -3552,7 +3837,7 @@
     <n v="5168.9395999999997"/>
   </r>
   <r>
-    <n v="2005"/>
+    <x v="9"/>
     <x v="2"/>
     <x v="2"/>
     <n v="2781878"/>
@@ -3561,7 +3846,7 @@
     <n v="2813.7559999999999"/>
   </r>
   <r>
-    <n v="2006"/>
+    <x v="10"/>
     <x v="7"/>
     <x v="2"/>
     <n v="3923198.4092827002"/>
@@ -3570,7 +3855,7 @@
     <n v="1734.8665471167401"/>
   </r>
   <r>
-    <n v="2006"/>
+    <x v="10"/>
     <x v="35"/>
     <x v="2"/>
     <n v="8642187.5021097101"/>
@@ -3579,7 +3864,7 @@
     <n v="8907.5158255977494"/>
   </r>
   <r>
-    <n v="2007"/>
+    <x v="1"/>
     <x v="7"/>
     <x v="2"/>
     <n v="3432559.42857143"/>
@@ -3588,7 +3873,7 @@
     <n v="3120.72683110654"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="36"/>
     <x v="0"/>
     <n v="10521654.704"/>
@@ -3597,7 +3882,7 @@
     <n v="5346.8962171428602"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="36"/>
     <x v="0"/>
     <n v="9244473"/>
@@ -3606,7 +3891,7 @@
     <n v="2746.0521428571401"/>
   </r>
   <r>
-    <n v="2003"/>
+    <x v="11"/>
     <x v="34"/>
     <x v="1"/>
     <n v="2746238.8373702401"/>
@@ -3615,7 +3900,7 @@
     <n v="5732.3601937716303"/>
   </r>
   <r>
-    <n v="2003"/>
+    <x v="11"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5748959.5617070403"/>
@@ -3624,7 +3909,7 @@
     <n v="6245.3239677047304"/>
   </r>
   <r>
-    <n v="2006"/>
+    <x v="10"/>
     <x v="22"/>
     <x v="2"/>
     <n v="5532421.4556962"/>
@@ -3633,7 +3918,7 @@
     <n v="1343.3374824191301"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="6"/>
     <x v="1"/>
     <n v="1829746.6"/>
@@ -3642,7 +3927,7 @@
     <n v="3063.15533333333"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="7"/>
     <x v="2"/>
     <n v="8440584.9879999999"/>
@@ -3651,7 +3936,7 @@
     <n v="9513.6416466666706"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5492478"/>
@@ -3660,7 +3945,7 @@
     <n v="6484.9560000000001"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="34"/>
     <x v="1"/>
     <n v="2746239"/>
@@ -3669,7 +3954,7 @@
     <n v="8484.9560000000001"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="34"/>
     <x v="1"/>
     <n v="2746239"/>
@@ -3678,7 +3963,7 @@
     <n v="8984.9560000000001"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="36"/>
     <x v="0"/>
     <n v="7468634.6863468597"/>
@@ -3687,7 +3972,7 @@
     <n v="3869.0195044807601"/>
   </r>
   <r>
-    <n v="2005"/>
+    <x v="9"/>
     <x v="2"/>
     <x v="2"/>
     <n v="3706532.5"/>
@@ -3696,7 +3981,7 @@
     <n v="4663.0649999999996"/>
   </r>
   <r>
-    <n v="2005"/>
+    <x v="9"/>
     <x v="23"/>
     <x v="0"/>
     <n v="5785903.2000000002"/>
@@ -3705,7 +3990,7 @@
     <n v="3310.9032000000002"/>
   </r>
   <r>
-    <n v="2006"/>
+    <x v="10"/>
     <x v="22"/>
     <x v="2"/>
     <n v="9310560.1265822798"/>
@@ -3714,7 +3999,7 @@
     <n v="5541.2693389592096"/>
   </r>
   <r>
-    <n v="2006"/>
+    <x v="10"/>
     <x v="31"/>
     <x v="0"/>
     <n v="4961575.5274261599"/>
@@ -3723,7 +4008,7 @@
     <n v="131.481715893108"/>
   </r>
   <r>
-    <n v="2008"/>
+    <x v="7"/>
     <x v="7"/>
     <x v="2"/>
     <n v="5805125.8064516103"/>
@@ -3732,7 +4017,7 @@
     <n v="5084.4838709677397"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="37"/>
     <x v="4"/>
     <n v="16221054"/>
@@ -3741,7 +4026,7 @@
     <n v="2757.5192857142902"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="36"/>
     <x v="0"/>
     <n v="8775645.7564575598"/>
@@ -3750,7 +4035,7 @@
     <n v="4802.5988402741204"/>
   </r>
   <r>
-    <n v="2014"/>
+    <x v="6"/>
     <x v="36"/>
     <x v="0"/>
     <n v="8775645.7564575598"/>
@@ -3759,7 +4044,7 @@
     <n v="3506.2572482867699"/>
   </r>
   <r>
-    <n v="2004"/>
+    <x v="8"/>
     <x v="23"/>
     <x v="0"/>
     <n v="7077062.7116049398"/>
@@ -3768,7 +4053,7 @@
     <n v="4246.23762469136"/>
   </r>
   <r>
-    <n v="2005"/>
+    <x v="9"/>
     <x v="2"/>
     <x v="2"/>
     <n v="3320046.4"/>
@@ -3777,7 +4062,7 @@
     <n v="3890.0927999999999"/>
   </r>
   <r>
-    <n v="2006"/>
+    <x v="10"/>
     <x v="2"/>
     <x v="2"/>
     <n v="5088204.6962025296"/>
@@ -3786,7 +4071,7 @@
     <n v="7507.63302109705"/>
   </r>
   <r>
-    <n v="2006"/>
+    <x v="10"/>
     <x v="34"/>
     <x v="1"/>
     <n v="2647234.00843882"/>
@@ -3795,7 +4080,7 @@
     <n v="7920.1596624472604"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="36"/>
     <x v="0"/>
     <n v="18495054.952"/>
@@ -3804,7 +4089,7 @@
     <n v="8909.7535371428603"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="6"/>
     <x v="1"/>
     <n v="2064000.3119999999"/>
@@ -3813,7 +4098,7 @@
     <n v="2326.0010400000001"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="37"/>
     <x v="4"/>
     <n v="17951730.368000001"/>
@@ -3822,7 +4107,7 @@
     <n v="3339.1894171428598"/>
   </r>
   <r>
-    <n v="2002"/>
+    <x v="12"/>
     <x v="7"/>
     <x v="2"/>
     <n v="5070748.63058824"/>
@@ -3831,7 +4116,7 @@
     <n v="5474.7771294117701"/>
   </r>
   <r>
-    <n v="2007"/>
+    <x v="1"/>
     <x v="3"/>
     <x v="1"/>
     <n v="1217062.6104830401"/>
@@ -3840,7 +4125,7 @@
     <n v="3485.1075025693699"/>
   </r>
   <r>
-    <n v="2009"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
     <n v="3377487.2560000001"/>
@@ -3849,7 +4134,7 @@
     <n v="5913.7181399999999"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="2968194"/>
@@ -3858,7 +4143,7 @@
     <n v="4920.4849999999997"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="3131505"/>
@@ -3867,7 +4152,7 @@
     <n v="5328.7624999999998"/>
   </r>
   <r>
-    <n v="2005"/>
+    <x v="9"/>
     <x v="3"/>
     <x v="1"/>
     <n v="1815958.1"/>
@@ -3876,7 +4161,7 @@
     <n v="6329.7905000000001"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="8"/>
     <x v="2"/>
     <n v="4860000"/>
@@ -3885,7 +4170,7 @@
     <n v="1575"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="8"/>
     <x v="2"/>
     <n v="11175690"/>
@@ -3894,7 +4179,7 @@
     <n v="11469.612499999999"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="1"/>
     <x v="1"/>
     <n v="3859524.0619554701"/>
@@ -3903,7 +4188,7 @@
     <n v="7444.5507163601196"/>
   </r>
   <r>
-    <n v="2012"/>
+    <x v="4"/>
     <x v="1"/>
     <x v="1"/>
     <n v="3357381.1863117898"/>
@@ -3912,7 +4197,7 @@
     <n v="6229.0042965779503"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="31"/>
     <x v="0"/>
     <n v="9010250"/>
@@ -3921,7 +4206,7 @@
     <n v="5216.875"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="31"/>
     <x v="0"/>
     <n v="7816000"/>
@@ -3930,7 +4215,7 @@
     <n v="4221.6666666666697"/>
   </r>
   <r>
-    <n v="2011"/>
+    <x v="3"/>
     <x v="1"/>
     <x v="1"/>
     <n v="3866770.6873184899"/>
@@ -3939,7 +4224,7 @@
     <n v="7462.6672797676702"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="2828428"/>
@@ -3948,7 +4233,7 @@
     <n v="2571.0700000000002"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="2829801"/>
@@ -3957,7 +4242,7 @@
     <n v="2574.5025000000001"/>
   </r>
   <r>
-    <n v="2010"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <n v="2873577"/>
@@ -3969,7 +4254,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -4039,7 +4324,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -4220,6 +4505,150 @@
   <dataFields count="1">
     <dataField name="Count of year" fld="0" subtotal="count" baseField="1" baseItem="0"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="14">
+        <item x="12"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="39">
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="34"/>
+        <item x="20"/>
+        <item x="6"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="17"/>
+        <item x="21"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="19"/>
+        <item x="2"/>
+        <item x="14"/>
+        <item x="7"/>
+        <item x="12"/>
+        <item x="24"/>
+        <item x="35"/>
+        <item x="25"/>
+        <item x="8"/>
+        <item x="16"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="31"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="18"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of capacity_kW" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -4594,8 +5023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4930,6 +5359,146 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B6" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B9" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B10" s="3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B11" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B12" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B14" s="3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G391"/>
   <sheetViews>
@@ -14334,28 +14903,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>